<commit_message>
better try catch logic and edge cases
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMA\SMA\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Smav2\SocialMediaAnalyser\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A7991B-0DDB-4C04-8930-8DDA67B7D05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75EE9AC-25DB-4737-A113-94879C417665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
     <t>test@test.com</t>
   </si>
   <si>
-    <t>https://www.tiktok.com/@selly,https://www.tiktok.com/@elianmita</t>
+    <t>https://www.tiktok.com/@elianmita,https://www.tiktok.com/@selly</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>